<commit_message>
base commit for summary pipeline
</commit_message>
<xml_diff>
--- a/data/audios_info/mapping.xlsx
+++ b/data/audios_info/mapping.xlsx
@@ -269,7 +269,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -283,6 +283,13 @@
     </fill>
   </fills>
   <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -305,29 +312,22 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -664,7 +664,7 @@
     <col min="12" max="12" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="21">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -700,7 +700,7 @@
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -732,7 +732,7 @@
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -770,7 +770,7 @@
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -844,7 +844,7 @@
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="3" t="s">
         <v>37</v>
       </c>
@@ -880,7 +880,7 @@
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="3" t="s">
         <v>43</v>
       </c>
@@ -918,7 +918,7 @@
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="3" t="s">
         <v>51</v>
       </c>
@@ -956,7 +956,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="3" t="s">
         <v>58</v>
       </c>
@@ -994,7 +994,7 @@
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="3" t="s">
         <v>64</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="21">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="3" t="s">
         <v>71</v>
       </c>

</xml_diff>